<commit_message>
clean folder, save changes
</commit_message>
<xml_diff>
--- a/datasets/from_translate/translatE_spanish_positives_112.xlsx
+++ b/datasets/from_translate/translatE_spanish_positives_112.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqvberde\Dropbox\TRANSLATE\ML\classifier\datasets\from_translate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqvberde/Projects/classifier_spanish/datasets/from_translate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0755F73-3D13-44C1-94E6-80DBD331389E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD448996-E7B8-F243-B50F-3440E3DB4235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83DE6F4E-0210-4630-8635-C86A9D49DCF4}"/>
+    <workbookView xWindow="860" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{83DE6F4E-0210-4630-8635-C86A9D49DCF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="1224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2243" uniqueCount="1224">
   <si>
     <t>Journal</t>
   </si>
@@ -4147,9 +4147,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4187,7 +4187,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4293,7 +4293,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4435,7 +4435,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4446,15 +4446,16 @@
   <dimension ref="A1:AB112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="31.140625" customWidth="1"/>
+    <col min="9" max="9" width="51.5" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1193</v>
       </c>
@@ -4540,7 +4541,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1218</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -4705,7 +4706,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>203</v>
       </c>
@@ -4788,7 +4789,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -4871,7 +4872,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>226</v>
       </c>
@@ -4948,7 +4949,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -5034,7 +5035,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>261</v>
       </c>
@@ -5200,7 +5201,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>276</v>
       </c>
@@ -5286,7 +5287,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>287</v>
       </c>
@@ -5369,7 +5370,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>297</v>
       </c>
@@ -5452,7 +5453,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>309</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>322</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>336</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>349</v>
       </c>
@@ -5781,7 +5782,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>359</v>
       </c>
@@ -5861,7 +5862,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>369</v>
       </c>
@@ -5947,7 +5948,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>383</v>
       </c>
@@ -6033,7 +6034,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>399</v>
       </c>
@@ -6119,7 +6120,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>416</v>
       </c>
@@ -6205,7 +6206,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>431</v>
       </c>
@@ -6279,7 +6280,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>443</v>
       </c>
@@ -6363,7 +6364,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>455</v>
       </c>
@@ -6444,7 +6445,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>465</v>
       </c>
@@ -6530,7 +6531,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>477</v>
       </c>
@@ -6613,7 +6614,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>490</v>
       </c>
@@ -6699,7 +6700,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>501</v>
       </c>
@@ -6783,7 +6784,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>512</v>
       </c>
@@ -6869,7 +6870,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>524</v>
       </c>
@@ -6955,7 +6956,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>534</v>
       </c>
@@ -7041,7 +7042,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>545</v>
       </c>
@@ -7127,7 +7128,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>556</v>
       </c>
@@ -7213,7 +7214,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>566</v>
       </c>
@@ -7299,7 +7300,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>576</v>
       </c>
@@ -7382,7 +7383,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>586</v>
       </c>
@@ -7468,7 +7469,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>597</v>
       </c>
@@ -7554,7 +7555,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>608</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>620</v>
       </c>
@@ -7726,7 +7727,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>634</v>
       </c>
@@ -7749,10 +7750,10 @@
         <v>2013</v>
       </c>
       <c r="H40" t="s">
+        <v>143</v>
+      </c>
+      <c r="I40" t="s">
         <v>636</v>
-      </c>
-      <c r="I40" t="s">
-        <v>143</v>
       </c>
       <c r="J40" t="s">
         <v>84</v>
@@ -7803,7 +7804,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>645</v>
       </c>
@@ -7884,7 +7885,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>656</v>
       </c>
@@ -7965,7 +7966,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>665</v>
       </c>
@@ -8043,7 +8044,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>675</v>
       </c>
@@ -8123,7 +8124,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>687</v>
       </c>
@@ -8194,7 +8195,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>699</v>
       </c>
@@ -8271,7 +8272,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>711</v>
       </c>
@@ -8348,7 +8349,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>724</v>
       </c>
@@ -8422,7 +8423,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>736</v>
       </c>
@@ -8496,7 +8497,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>748</v>
       </c>
@@ -8576,7 +8577,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>762</v>
       </c>
@@ -8654,7 +8655,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>775</v>
       </c>
@@ -8734,7 +8735,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>787</v>
       </c>
@@ -8757,10 +8758,10 @@
         <v>2016</v>
       </c>
       <c r="H53" t="s">
+        <v>156</v>
+      </c>
+      <c r="I53" t="s">
         <v>789</v>
-      </c>
-      <c r="I53" t="s">
-        <v>156</v>
       </c>
       <c r="J53" t="s">
         <v>89</v>
@@ -8817,7 +8818,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>799</v>
       </c>
@@ -8894,7 +8895,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>811</v>
       </c>
@@ -8980,7 +8981,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>828</v>
       </c>
@@ -9060,7 +9061,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>841</v>
       </c>
@@ -9140,7 +9141,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>855</v>
       </c>
@@ -9226,7 +9227,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>869</v>
       </c>
@@ -9306,7 +9307,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>880</v>
       </c>
@@ -9389,7 +9390,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>893</v>
       </c>
@@ -9466,7 +9467,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>904</v>
       </c>
@@ -9546,7 +9547,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>915</v>
       </c>
@@ -9632,7 +9633,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>926</v>
       </c>
@@ -9712,7 +9713,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>937</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>949</v>
       </c>
@@ -9878,7 +9879,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>961</v>
       </c>
@@ -9958,7 +9959,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>972</v>
       </c>
@@ -10035,7 +10036,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>983</v>
       </c>
@@ -10115,7 +10116,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>994</v>
       </c>
@@ -10195,7 +10196,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1006</v>
       </c>
@@ -10281,7 +10282,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1020</v>
       </c>
@@ -10355,7 +10356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1032</v>
       </c>
@@ -10432,7 +10433,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1043</v>
       </c>
@@ -10509,7 +10510,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>1054</v>
       </c>
@@ -10592,7 +10593,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1065</v>
       </c>
@@ -10669,7 +10670,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1078</v>
       </c>
@@ -10743,7 +10744,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1088</v>
       </c>
@@ -10820,7 +10821,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1097</v>
       </c>
@@ -10892,7 +10893,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1107</v>
       </c>
@@ -10911,12 +10912,6 @@
       <c r="G80">
         <v>2006</v>
       </c>
-      <c r="H80" t="s">
-        <v>325</v>
-      </c>
-      <c r="I80" t="s">
-        <v>325</v>
-      </c>
       <c r="J80" t="s">
         <v>100</v>
       </c>
@@ -10942,7 +10937,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1115</v>
       </c>
@@ -10961,12 +10956,6 @@
       <c r="G81">
         <v>2006</v>
       </c>
-      <c r="H81" t="s">
-        <v>325</v>
-      </c>
-      <c r="I81" t="s">
-        <v>325</v>
-      </c>
       <c r="J81" t="s">
         <v>100</v>
       </c>
@@ -10992,7 +10981,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1118</v>
       </c>
@@ -11011,12 +11000,6 @@
       <c r="G82">
         <v>2006</v>
       </c>
-      <c r="H82" t="s">
-        <v>325</v>
-      </c>
-      <c r="I82" t="s">
-        <v>325</v>
-      </c>
       <c r="J82" t="s">
         <v>100</v>
       </c>
@@ -11042,7 +11025,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1120</v>
       </c>
@@ -11061,12 +11044,6 @@
       <c r="G83">
         <v>2006</v>
       </c>
-      <c r="H83" t="s">
-        <v>325</v>
-      </c>
-      <c r="I83" t="s">
-        <v>325</v>
-      </c>
       <c r="J83" t="s">
         <v>100</v>
       </c>
@@ -11092,7 +11069,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1122</v>
       </c>
@@ -11111,12 +11088,6 @@
       <c r="G84">
         <v>2006</v>
       </c>
-      <c r="H84" t="s">
-        <v>325</v>
-      </c>
-      <c r="I84" t="s">
-        <v>325</v>
-      </c>
       <c r="J84" t="s">
         <v>100</v>
       </c>
@@ -11142,7 +11113,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1124</v>
       </c>
@@ -11161,12 +11132,6 @@
       <c r="G85">
         <v>2006</v>
       </c>
-      <c r="H85" t="s">
-        <v>325</v>
-      </c>
-      <c r="I85" t="s">
-        <v>325</v>
-      </c>
       <c r="J85" t="s">
         <v>100</v>
       </c>
@@ -11192,7 +11157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1126</v>
       </c>
@@ -11211,12 +11176,6 @@
       <c r="G86">
         <v>2006</v>
       </c>
-      <c r="H86" t="s">
-        <v>325</v>
-      </c>
-      <c r="I86" t="s">
-        <v>325</v>
-      </c>
       <c r="J86" t="s">
         <v>100</v>
       </c>
@@ -11242,7 +11201,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1128</v>
       </c>
@@ -11261,12 +11220,6 @@
       <c r="G87">
         <v>2006</v>
       </c>
-      <c r="H87" t="s">
-        <v>325</v>
-      </c>
-      <c r="I87" t="s">
-        <v>325</v>
-      </c>
       <c r="J87" t="s">
         <v>100</v>
       </c>
@@ -11292,7 +11245,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1130</v>
       </c>
@@ -11311,12 +11264,6 @@
       <c r="G88">
         <v>2006</v>
       </c>
-      <c r="H88" t="s">
-        <v>325</v>
-      </c>
-      <c r="I88" t="s">
-        <v>325</v>
-      </c>
       <c r="J88" t="s">
         <v>100</v>
       </c>
@@ -11342,7 +11289,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1132</v>
       </c>
@@ -11361,12 +11308,6 @@
       <c r="G89">
         <v>2006</v>
       </c>
-      <c r="H89" t="s">
-        <v>325</v>
-      </c>
-      <c r="I89" t="s">
-        <v>325</v>
-      </c>
       <c r="J89" t="s">
         <v>100</v>
       </c>
@@ -11392,7 +11333,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1134</v>
       </c>
@@ -11411,12 +11352,6 @@
       <c r="G90">
         <v>2006</v>
       </c>
-      <c r="H90" t="s">
-        <v>325</v>
-      </c>
-      <c r="I90" t="s">
-        <v>325</v>
-      </c>
       <c r="J90" t="s">
         <v>100</v>
       </c>
@@ -11442,7 +11377,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1136</v>
       </c>
@@ -11461,12 +11396,6 @@
       <c r="G91">
         <v>2006</v>
       </c>
-      <c r="H91" t="s">
-        <v>325</v>
-      </c>
-      <c r="I91" t="s">
-        <v>325</v>
-      </c>
       <c r="J91" t="s">
         <v>100</v>
       </c>
@@ -11492,7 +11421,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1138</v>
       </c>
@@ -11511,12 +11440,6 @@
       <c r="G92">
         <v>2006</v>
       </c>
-      <c r="H92" t="s">
-        <v>325</v>
-      </c>
-      <c r="I92" t="s">
-        <v>325</v>
-      </c>
       <c r="J92" t="s">
         <v>100</v>
       </c>
@@ -11542,7 +11465,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>1140</v>
       </c>
@@ -11561,12 +11484,6 @@
       <c r="G93">
         <v>2006</v>
       </c>
-      <c r="H93" t="s">
-        <v>325</v>
-      </c>
-      <c r="I93" t="s">
-        <v>325</v>
-      </c>
       <c r="J93" t="s">
         <v>100</v>
       </c>
@@ -11592,7 +11509,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>1142</v>
       </c>
@@ -11611,12 +11528,6 @@
       <c r="G94">
         <v>2006</v>
       </c>
-      <c r="H94" t="s">
-        <v>325</v>
-      </c>
-      <c r="I94" t="s">
-        <v>325</v>
-      </c>
       <c r="J94" t="s">
         <v>100</v>
       </c>
@@ -11636,7 +11547,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1143</v>
       </c>
@@ -11655,12 +11566,6 @@
       <c r="G95">
         <v>2006</v>
       </c>
-      <c r="H95" t="s">
-        <v>325</v>
-      </c>
-      <c r="I95" t="s">
-        <v>325</v>
-      </c>
       <c r="J95" t="s">
         <v>100</v>
       </c>
@@ -11686,7 +11591,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1146</v>
       </c>
@@ -11705,12 +11610,6 @@
       <c r="G96">
         <v>2006</v>
       </c>
-      <c r="H96" t="s">
-        <v>325</v>
-      </c>
-      <c r="I96" t="s">
-        <v>325</v>
-      </c>
       <c r="J96" t="s">
         <v>100</v>
       </c>
@@ -11736,7 +11635,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>1149</v>
       </c>
@@ -11755,12 +11654,6 @@
       <c r="G97">
         <v>1995</v>
       </c>
-      <c r="H97" t="s">
-        <v>325</v>
-      </c>
-      <c r="I97" t="s">
-        <v>325</v>
-      </c>
       <c r="J97" t="s">
         <v>101</v>
       </c>
@@ -11786,7 +11679,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>1155</v>
       </c>
@@ -11805,12 +11698,6 @@
       <c r="G98">
         <v>1995</v>
       </c>
-      <c r="H98" t="s">
-        <v>325</v>
-      </c>
-      <c r="I98" t="s">
-        <v>325</v>
-      </c>
       <c r="J98" t="s">
         <v>101</v>
       </c>
@@ -11836,7 +11723,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>1157</v>
       </c>
@@ -11855,12 +11742,6 @@
       <c r="G99">
         <v>1995</v>
       </c>
-      <c r="H99" t="s">
-        <v>325</v>
-      </c>
-      <c r="I99" t="s">
-        <v>325</v>
-      </c>
       <c r="J99" t="s">
         <v>101</v>
       </c>
@@ -11886,7 +11767,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>1159</v>
       </c>
@@ -11905,12 +11786,6 @@
       <c r="G100">
         <v>1995</v>
       </c>
-      <c r="H100" t="s">
-        <v>325</v>
-      </c>
-      <c r="I100" t="s">
-        <v>325</v>
-      </c>
       <c r="J100" t="s">
         <v>101</v>
       </c>
@@ -11936,7 +11811,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>1161</v>
       </c>
@@ -11955,12 +11830,6 @@
       <c r="G101">
         <v>1995</v>
       </c>
-      <c r="H101" t="s">
-        <v>325</v>
-      </c>
-      <c r="I101" t="s">
-        <v>325</v>
-      </c>
       <c r="J101" t="s">
         <v>101</v>
       </c>
@@ -11986,7 +11855,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>1163</v>
       </c>
@@ -12005,12 +11874,6 @@
       <c r="G102">
         <v>1995</v>
       </c>
-      <c r="H102" t="s">
-        <v>325</v>
-      </c>
-      <c r="I102" t="s">
-        <v>325</v>
-      </c>
       <c r="J102" t="s">
         <v>101</v>
       </c>
@@ -12036,7 +11899,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>1166</v>
       </c>
@@ -12055,12 +11918,6 @@
       <c r="G103">
         <v>1995</v>
       </c>
-      <c r="H103" t="s">
-        <v>325</v>
-      </c>
-      <c r="I103" t="s">
-        <v>325</v>
-      </c>
       <c r="J103" t="s">
         <v>101</v>
       </c>
@@ -12086,7 +11943,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>1168</v>
       </c>
@@ -12105,12 +11962,6 @@
       <c r="G104">
         <v>1995</v>
       </c>
-      <c r="H104" t="s">
-        <v>325</v>
-      </c>
-      <c r="I104" t="s">
-        <v>325</v>
-      </c>
       <c r="J104" t="s">
         <v>101</v>
       </c>
@@ -12136,7 +11987,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>1170</v>
       </c>
@@ -12155,12 +12006,6 @@
       <c r="G105">
         <v>1995</v>
       </c>
-      <c r="H105" t="s">
-        <v>325</v>
-      </c>
-      <c r="I105" t="s">
-        <v>325</v>
-      </c>
       <c r="J105" t="s">
         <v>101</v>
       </c>
@@ -12186,7 +12031,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1172</v>
       </c>
@@ -12205,12 +12050,6 @@
       <c r="G106">
         <v>1995</v>
       </c>
-      <c r="H106" t="s">
-        <v>325</v>
-      </c>
-      <c r="I106" t="s">
-        <v>325</v>
-      </c>
       <c r="J106" t="s">
         <v>101</v>
       </c>
@@ -12236,7 +12075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>1174</v>
       </c>
@@ -12255,12 +12094,6 @@
       <c r="G107">
         <v>1995</v>
       </c>
-      <c r="H107" t="s">
-        <v>325</v>
-      </c>
-      <c r="I107" t="s">
-        <v>325</v>
-      </c>
       <c r="J107" t="s">
         <v>101</v>
       </c>
@@ -12286,7 +12119,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1176</v>
       </c>
@@ -12305,12 +12138,6 @@
       <c r="G108">
         <v>2009</v>
       </c>
-      <c r="H108" t="s">
-        <v>325</v>
-      </c>
-      <c r="I108" t="s">
-        <v>325</v>
-      </c>
       <c r="J108" t="s">
         <v>102</v>
       </c>
@@ -12330,7 +12157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>1180</v>
       </c>
@@ -12349,12 +12176,6 @@
       <c r="G109">
         <v>2002</v>
       </c>
-      <c r="H109" t="s">
-        <v>325</v>
-      </c>
-      <c r="I109" t="s">
-        <v>325</v>
-      </c>
       <c r="J109" t="s">
         <v>102</v>
       </c>
@@ -12374,7 +12195,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>1184</v>
       </c>
@@ -12393,12 +12214,6 @@
       <c r="G110">
         <v>2015</v>
       </c>
-      <c r="H110" t="s">
-        <v>325</v>
-      </c>
-      <c r="I110" t="s">
-        <v>325</v>
-      </c>
       <c r="J110" t="s">
         <v>103</v>
       </c>
@@ -12418,7 +12233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>1188</v>
       </c>
@@ -12437,12 +12252,6 @@
       <c r="G111">
         <v>2015</v>
       </c>
-      <c r="H111" t="s">
-        <v>325</v>
-      </c>
-      <c r="I111" t="s">
-        <v>325</v>
-      </c>
       <c r="J111" t="s">
         <v>103</v>
       </c>
@@ -12462,7 +12271,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1189</v>
       </c>
@@ -12480,12 +12289,6 @@
       </c>
       <c r="G112">
         <v>2003</v>
-      </c>
-      <c r="H112" t="s">
-        <v>325</v>
-      </c>
-      <c r="I112" t="s">
-        <v>325</v>
       </c>
       <c r="J112" t="s">
         <v>99</v>

</xml_diff>